<commit_message>
Edited issue spreadsheet, formatting SRS
</commit_message>
<xml_diff>
--- a/Documents/Status Updates/StatusSheet.xlsx
+++ b/Documents/Status Updates/StatusSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15880" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15880" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>This is an example</t>
+  </si>
+  <si>
+    <t>Projected Resolution Date</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +262,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -598,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -945,19 +949,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="46.1640625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,8 +975,11 @@
       <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -983,6 +991,9 @@
       </c>
       <c r="D2" t="s">
         <v>51</v>
+      </c>
+      <c r="E2" s="5">
+        <v>41564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formatting mentioned in class
</commit_message>
<xml_diff>
--- a/Documents/Status Updates/StatusSheet.xlsx
+++ b/Documents/Status Updates/StatusSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Number</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>Projected Resolution Date</t>
+  </si>
+  <si>
+    <t>Customer MIA</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>New customer acquired</t>
   </si>
 </sst>
 </file>
@@ -949,16 +958,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="46.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -994,6 +1003,23 @@
       </c>
       <c r="E2" s="5">
         <v>41564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="5">
+        <v>41559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formatting, SDD Requirements Matrix, minor edits, signoff page
Added a new sheet to the ongoing status sheet. "Functional Flow Table"
fulfills the requirements for the Requirements Matrix.
</commit_message>
<xml_diff>
--- a/Documents/Status Updates/StatusSheet.xlsx
+++ b/Documents/Status Updates/StatusSheet.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15880" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22900" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="Deliverables" sheetId="2" r:id="rId2"/>
-    <sheet name="Issues" sheetId="3" r:id="rId3"/>
+    <sheet name="Functional Flow Table" sheetId="4" r:id="rId2"/>
+    <sheet name="Deliverables" sheetId="2" r:id="rId3"/>
+    <sheet name="Issues" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
   <si>
     <t>Number</t>
   </si>
@@ -47,15 +48,6 @@
     <t>Admins shall be able to edit sites</t>
   </si>
   <si>
-    <t>1.2.2</t>
-  </si>
-  <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
     <t>Section 2</t>
   </si>
   <si>
@@ -192,6 +184,183 @@
   </si>
   <si>
     <t>Date of Completion</t>
+  </si>
+  <si>
+    <t>Requirement Name</t>
+  </si>
+  <si>
+    <t>Requirement #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Display visually the window of operation to the user.</t>
+  </si>
+  <si>
+    <t>Modifies the GUI to allow interactions based on user permissions. Requires the input of a known username/password combination</t>
+  </si>
+  <si>
+    <t>Reverts the GUI to initial state, removing all interactions except the option to input a username and password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Setup</t>
+  </si>
+  <si>
+    <t>User Interaction</t>
+  </si>
+  <si>
+    <t>SelectStart</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>SelectEnd</t>
+  </si>
+  <si>
+    <t>2.4.1</t>
+  </si>
+  <si>
+    <t>2.4.2</t>
+  </si>
+  <si>
+    <t>2.4.3</t>
+  </si>
+  <si>
+    <t>DisplayHelp</t>
+  </si>
+  <si>
+    <t>CalculateRoute</t>
+  </si>
+  <si>
+    <t>DisplayRoute</t>
+  </si>
+  <si>
+    <t>GenerateWaypointList</t>
+  </si>
+  <si>
+    <t>CalculateDistance</t>
+  </si>
+  <si>
+    <t>The user chooses a start waypoint, and the system flags this as the starting location in route calculations.</t>
+  </si>
+  <si>
+    <t>The user chooses an end waypoint, and the system flags this as the final location in route calculations.</t>
+  </si>
+  <si>
+    <t>The user inputs a name, lat/long coordinate pair and description for a new waypoint, which is then stored in the database.</t>
+  </si>
+  <si>
+    <t>AddWaypoint (ADMIN)</t>
+  </si>
+  <si>
+    <t>RemoveWaypoint (ADMIN)</t>
+  </si>
+  <si>
+    <t>EditWaypoint (ADMIN)</t>
+  </si>
+  <si>
+    <t>ChangeName (ADMIN)</t>
+  </si>
+  <si>
+    <t>ChangeCoordinates (ADMIN)</t>
+  </si>
+  <si>
+    <t>ChangeDescription (ADMIN)</t>
+  </si>
+  <si>
+    <t>The user selects a waypoint by name, and upon confirmation this waypoint is removed from the database.</t>
+  </si>
+  <si>
+    <t>The user selects a waypoint by name, and a new panel appears in the GUI to edit the details of this waypoint.</t>
+  </si>
+  <si>
+    <t>The user inputs a new name for the waypoint, which is then changed in the GUI and database.</t>
+  </si>
+  <si>
+    <t>The user inputs a new lat/long coordinate pair for the waypoint, which is then changed in the GUI and database.</t>
+  </si>
+  <si>
+    <t>The user inputs a new description for the waypoint, which is then changed in the GUI and database.</t>
+  </si>
+  <si>
+    <t>Upon selection of this option, the user will be shown a help file with detailed information on all available functions for their permission level.</t>
+  </si>
+  <si>
+    <t>The system calculates the shortest straight-line path between every waypoint in the list, starting at the selected start and terminating at the selected end.</t>
+  </si>
+  <si>
+    <t>The system queries Google Earth to display the calculated route.</t>
+  </si>
+  <si>
+    <t>The system pulls all available waypoints from the database to provide a list to the user.</t>
+  </si>
+  <si>
+    <t>The system calculates the total distance of the route based on lat/long changes.</t>
+  </si>
+  <si>
+    <t>Functions required for basic interaction</t>
+  </si>
+  <si>
+    <t>Functions outside of Section 1 that require a user trigger.</t>
+  </si>
+  <si>
+    <t>Functions that act within the syste, without user interaction.</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Logoff</t>
+  </si>
+  <si>
+    <t>LoadGUI</t>
+  </si>
+  <si>
+    <t>Logs in</t>
+  </si>
+  <si>
+    <t>Logs off</t>
+  </si>
+  <si>
+    <t>Edit location information</t>
+  </si>
+  <si>
+    <t>Find Distance</t>
+  </si>
+  <si>
+    <t>Calculate Route</t>
+  </si>
+  <si>
+    <t>Display Route</t>
+  </si>
+  <si>
+    <t>Get Help</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>Show Waypoints</t>
+  </si>
+  <si>
+    <t>Edit waypoint information</t>
+  </si>
+  <si>
+    <t>Prompt waypoints</t>
+  </si>
+  <si>
+    <t>Deletes waypoint</t>
+  </si>
+  <si>
+    <t>Adds waypoint</t>
+  </si>
+  <si>
+    <t>Show GUI</t>
   </si>
 </sst>
 </file>
@@ -255,7 +424,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -263,26 +432,82 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -615,187 +840,190 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="61.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="11"/>
+    <col min="2" max="2" width="61.6640625" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3">
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="10">
+        <v>2.4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="11">
+        <v>3.1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45">
+      <c r="A13" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="11">
+        <v>3.6</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>2.1</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="11">
+        <v>3.8</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>3.1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>3.2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>3.3</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="11">
+        <v>3.9</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="5" customFormat="1">
+      <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>3.4</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>3.5</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>3.6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>3.7</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>3.8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>3.9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="2" customFormat="1">
-      <c r="A22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>4.2</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -806,9 +1034,360 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="18"/>
+    <col min="2" max="2" width="24.6640625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="24.5" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="12" customFormat="1">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="30">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60">
+      <c r="A4" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60">
+      <c r="A5" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="16" customFormat="1" ht="30">
+      <c r="A7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="13">
+        <v>3.1</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60">
+      <c r="A10" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="18">
+        <v>2.4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60">
+      <c r="A14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45">
+      <c r="A15" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="16" customFormat="1" ht="30">
+      <c r="A17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60">
+      <c r="A18" s="18">
+        <v>3.1</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="75">
+      <c r="A19" s="18">
+        <v>3.2</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20" s="18">
+        <v>3.3</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="13">
+        <v>4.3</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45">
+      <c r="A21" s="18">
+        <v>3.4</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45">
+      <c r="A22" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="13">
+        <v>4.2</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -825,19 +1404,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1">
@@ -845,10 +1424,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -856,7 +1435,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -864,10 +1443,10 @@
         <v>1.2</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -875,24 +1454,24 @@
         <v>1.3</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
         <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -900,7 +1479,7 @@
         <v>2.1</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -908,10 +1487,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -919,10 +1498,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -930,10 +1509,10 @@
         <v>2.4</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -941,7 +1520,7 @@
         <v>2.5</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -949,7 +1528,7 @@
         <v>2.6</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +1542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -983,16 +1562,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1000,15 +1579,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="5">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3">
         <v>41564</v>
       </c>
     </row>
@@ -1017,15 +1596,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="5">
+        <v>52</v>
+      </c>
+      <c r="E3" s="3">
         <v>41559</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added known GUI defects to StatusSheet
</commit_message>
<xml_diff>
--- a/Documents/Status Updates/StatusSheet.xlsx
+++ b/Documents/Status Updates/StatusSheet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\GitHub\UMBC-CMSC_345_TWIX\Documents\Status Updates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22900" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="16065" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <author>Stephen Moore</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="165">
   <si>
     <t>Number</t>
   </si>
@@ -562,6 +567,27 @@
   </si>
   <si>
     <t>Section ID</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Logout Functionality</t>
+  </si>
+  <si>
+    <t>"Log Out" button on GUI does not perform any functions.</t>
+  </si>
+  <si>
+    <t>Color Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement of blue and green GUI is not met. </t>
+  </si>
+  <si>
+    <t>Validation of Additions</t>
+  </si>
+  <si>
+    <t>When administrators add new users or locations, there is no notification of how duplicates are handled from the client side.</t>
   </si>
 </sst>
 </file>
@@ -667,7 +693,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,6 +781,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -774,6 +809,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1105,14 +1148,14 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="11"/>
-    <col min="2" max="2" width="61.6640625" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="10.875" style="11"/>
+    <col min="2" max="2" width="61.625" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -1131,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1.1000000000000001</v>
       </c>
@@ -1139,7 +1182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -1147,7 +1190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>2.1</v>
       </c>
@@ -1155,7 +1198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2.2000000000000002</v>
       </c>
@@ -1163,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>2.2999999999999998</v>
       </c>
@@ -1171,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2.4</v>
       </c>
@@ -1179,7 +1222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1230,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>3.1</v>
       </c>
@@ -1195,7 +1238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>3.2</v>
       </c>
@@ -1203,7 +1246,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>3.3</v>
       </c>
@@ -1211,7 +1254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>3.4</v>
       </c>
@@ -1219,7 +1262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>3.5</v>
       </c>
@@ -1227,7 +1270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>3.6</v>
       </c>
@@ -1235,7 +1278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>3.7</v>
       </c>
@@ -1243,7 +1286,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3.8</v>
       </c>
@@ -1251,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>3.9</v>
       </c>
@@ -1259,7 +1302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="5" customFormat="1">
+    <row r="22" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1267,7 +1310,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -1275,7 +1318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>4.2</v>
       </c>
@@ -1302,17 +1345,17 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="18"/>
-    <col min="2" max="2" width="24.6640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="18"/>
+    <col min="2" max="2" width="24.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="32.125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="21.125" style="13" customWidth="1"/>
     <col min="5" max="5" width="24.5" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="13"/>
+    <col min="6" max="16384" width="10.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1329,7 +1372,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" ht="30">
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
@@ -1340,7 +1383,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1.1000000000000001</v>
       </c>
@@ -1357,7 +1400,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>1.2</v>
       </c>
@@ -1374,7 +1417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60">
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>1.3</v>
       </c>
@@ -1391,7 +1434,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="16" customFormat="1" ht="30">
+    <row r="7" spans="1:5" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
@@ -1402,7 +1445,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45">
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>63</v>
       </c>
@@ -1419,7 +1462,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45">
+    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>64</v>
       </c>
@@ -1436,7 +1479,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60">
+    <row r="10" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>2.2000000000000002</v>
       </c>
@@ -1453,7 +1496,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>2.2999999999999998</v>
       </c>
@@ -1470,7 +1513,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="45">
+    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>2.4</v>
       </c>
@@ -1487,7 +1530,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45">
+    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>66</v>
       </c>
@@ -1504,7 +1547,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60">
+    <row r="14" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>67</v>
       </c>
@@ -1521,7 +1564,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>68</v>
       </c>
@@ -1538,7 +1581,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="16" customFormat="1" ht="30">
+    <row r="17" spans="1:5" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>10</v>
       </c>
@@ -1549,7 +1592,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60">
+    <row r="18" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>3.1</v>
       </c>
@@ -1566,7 +1609,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="75">
+    <row r="19" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>3.2</v>
       </c>
@@ -1583,7 +1626,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30">
+    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>3.3</v>
       </c>
@@ -1600,7 +1643,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45">
+    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>3.4</v>
       </c>
@@ -1617,7 +1660,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45">
+    <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>3.5</v>
       </c>
@@ -1653,15 +1696,15 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
     <col min="4" max="5" width="19.5" customWidth="1"/>
     <col min="6" max="6" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1692,7 +1735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1700,7 +1743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -1711,7 +1754,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -1722,7 +1765,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1736,7 +1779,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.1</v>
       </c>
@@ -1744,7 +1787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
@@ -1755,7 +1798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
@@ -1766,7 +1809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.4</v>
       </c>
@@ -1777,7 +1820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.5</v>
       </c>
@@ -1785,7 +1828,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.6</v>
       </c>
@@ -1812,14 +1855,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="46.125" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1879,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1853,7 +1896,7 @@
         <v>41564</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1889,19 +1932,19 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1915,12 +1958,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1945,21 +1988,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="21"/>
-    <col min="2" max="2" width="26.83203125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="21"/>
+    <col min="1" max="1" width="10.875" style="21"/>
+    <col min="2" max="2" width="26.875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="19.875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="32.375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="32.625" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="22" customFormat="1">
+    <row r="1" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>127</v>
       </c>
@@ -1973,7 +2016,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="23" customFormat="1">
+    <row r="2" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23">
         <v>1.1000000000000001</v>
       </c>
@@ -1987,7 +2030,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1.2</v>
       </c>
@@ -1998,7 +2041,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>1.3</v>
       </c>
@@ -2009,7 +2052,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="23" customFormat="1" ht="30">
+    <row r="5" spans="1:4" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <v>2.1</v>
       </c>
@@ -2023,7 +2066,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>2.2000000000000002</v>
       </c>
@@ -2034,7 +2077,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>2.2999999999999998</v>
       </c>
@@ -2045,7 +2088,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>2.4</v>
       </c>
@@ -2056,7 +2099,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="23" customFormat="1" ht="30">
+    <row r="9" spans="1:4" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>3.1</v>
       </c>
@@ -2070,7 +2113,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>3.2</v>
       </c>
@@ -2081,7 +2124,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>3.3</v>
       </c>
@@ -2092,7 +2135,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>3.4</v>
       </c>
@@ -2103,7 +2146,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="23" customFormat="1" ht="45">
+    <row r="13" spans="1:4" s="23" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>4.0999999999999996</v>
       </c>
@@ -2117,7 +2160,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>4.2</v>
       </c>
@@ -2128,7 +2171,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="23" customFormat="1" ht="30">
+    <row r="15" spans="1:4" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <v>5.0999999999999996</v>
       </c>
@@ -2142,7 +2185,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>5.2</v>
       </c>
@@ -2165,31 +2208,79 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.25" style="32" customWidth="1"/>
+    <col min="2" max="2" width="27.625" style="34" customWidth="1"/>
+    <col min="3" max="4" width="11" style="32"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="12" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="32">
+        <v>2.1</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="32">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="32">
+        <v>3.1</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added discovered route calculation defect
</commit_message>
<xml_diff>
--- a/Documents/Status Updates/StatusSheet.xlsx
+++ b/Documents/Status Updates/StatusSheet.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\GitHub\UMBC-CMSC_345_TWIX\Documents\Status Updates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="16065" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21720" windowHeight="13620" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -20,12 +15,7 @@
     <sheet name="Defect Checklist" sheetId="6" r:id="rId6"/>
     <sheet name="Defects Found" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="114210" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -35,7 +25,7 @@
     <author>Stephen Moore</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="167">
   <si>
     <t>Number</t>
   </si>
@@ -588,13 +578,19 @@
   </si>
   <si>
     <t>When administrators add new users or locations, there is no notification of how duplicates are handled from the client side.</t>
+  </si>
+  <si>
+    <t>Route calculated is not the shortest possible path</t>
+  </si>
+  <si>
+    <t>Correctness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -605,38 +601,19 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -672,26 +649,14 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -758,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -792,31 +757,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1141,21 +1086,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B1" sqref="B1:B65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" style="11"/>
     <col min="2" max="2" width="61.625" style="6" customWidth="1"/>
     <col min="3" max="16384" width="10.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +1111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -1174,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="31.5">
       <c r="A3" s="10">
         <v>1.1000000000000001</v>
       </c>
@@ -1182,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -1190,7 +1135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="11">
         <v>2.1</v>
       </c>
@@ -1198,7 +1143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="10">
         <v>2.2000000000000002</v>
       </c>
@@ -1206,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="10">
         <v>2.2999999999999998</v>
       </c>
@@ -1214,7 +1159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="10">
         <v>2.4</v>
       </c>
@@ -1222,7 +1167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1230,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="11">
         <v>3.1</v>
       </c>
@@ -1238,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="47.25">
       <c r="A13" s="11">
         <v>3.2</v>
       </c>
@@ -1246,7 +1191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="11">
         <v>3.3</v>
       </c>
@@ -1254,7 +1199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="11">
         <v>3.4</v>
       </c>
@@ -1262,7 +1207,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="31.5">
       <c r="A16" s="11">
         <v>3.5</v>
       </c>
@@ -1270,7 +1215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="11">
         <v>3.6</v>
       </c>
@@ -1278,7 +1223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="11">
         <v>3.7</v>
       </c>
@@ -1286,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="11">
         <v>3.8</v>
       </c>
@@ -1294,7 +1239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="11">
         <v>3.9</v>
       </c>
@@ -1302,7 +1247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="5" customFormat="1">
       <c r="A22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1310,7 +1255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -1318,7 +1263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="11">
         <v>4.2</v>
       </c>
@@ -1327,25 +1272,21 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" style="18"/>
     <col min="2" max="2" width="24.625" style="13" customWidth="1"/>
@@ -1355,7 +1296,7 @@
     <col min="6" max="16384" width="10.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="12" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1313,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="31.5">
       <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
@@ -1383,7 +1324,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="31.5">
       <c r="A3" s="18">
         <v>1.1000000000000001</v>
       </c>
@@ -1400,7 +1341,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="78.75">
       <c r="A4" s="18">
         <v>1.2</v>
       </c>
@@ -1417,7 +1358,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="63">
       <c r="A5" s="18">
         <v>1.3</v>
       </c>
@@ -1434,7 +1375,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="16" customFormat="1" ht="31.5">
       <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
@@ -1445,7 +1386,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="63">
       <c r="A8" s="18" t="s">
         <v>63</v>
       </c>
@@ -1462,7 +1403,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="47.25">
       <c r="A9" s="18" t="s">
         <v>64</v>
       </c>
@@ -1479,7 +1420,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="63">
       <c r="A10" s="18">
         <v>2.2000000000000002</v>
       </c>
@@ -1496,7 +1437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="47.25">
       <c r="A11" s="18">
         <v>2.2999999999999998</v>
       </c>
@@ -1513,7 +1454,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="47.25">
       <c r="A12" s="18">
         <v>2.4</v>
       </c>
@@ -1530,7 +1471,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="47.25">
       <c r="A13" s="18" t="s">
         <v>66</v>
       </c>
@@ -1547,7 +1488,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="63">
       <c r="A14" s="18" t="s">
         <v>67</v>
       </c>
@@ -1564,7 +1505,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="47.25">
       <c r="A15" s="18" t="s">
         <v>68</v>
       </c>
@@ -1581,7 +1522,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="16" customFormat="1" ht="31.5">
       <c r="A17" s="17" t="s">
         <v>10</v>
       </c>
@@ -1592,7 +1533,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="63">
       <c r="A18" s="18">
         <v>3.1</v>
       </c>
@@ -1609,7 +1550,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="78.75">
       <c r="A19" s="18">
         <v>3.2</v>
       </c>
@@ -1626,7 +1567,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="31.5">
       <c r="A20" s="18">
         <v>3.3</v>
       </c>
@@ -1643,7 +1584,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="47.25">
       <c r="A21" s="18">
         <v>3.4</v>
       </c>
@@ -1660,7 +1601,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="47.25">
       <c r="A22" s="18">
         <v>3.5</v>
       </c>
@@ -1678,25 +1619,21 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="12.375" customWidth="1"/>
@@ -1704,7 +1641,7 @@
     <col min="6" max="6" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1735,7 +1672,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1743,7 +1680,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -1754,7 +1691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -1765,7 +1702,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1779,7 +1716,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2.1</v>
       </c>
@@ -1787,7 +1724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
@@ -1798,7 +1735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
@@ -1809,7 +1746,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2.4</v>
       </c>
@@ -1820,7 +1757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2.5</v>
       </c>
@@ -1828,7 +1765,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2.6</v>
       </c>
@@ -1837,32 +1774,28 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="46.125" customWidth="1"/>
     <col min="4" max="4" width="21.125" customWidth="1"/>
     <col min="5" max="5" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +1812,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1896,7 +1829,7 @@
         <v>41564</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1914,37 +1847,33 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="23.625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1958,12 +1887,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1975,24 +1904,20 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" style="21"/>
     <col min="2" max="2" width="26.875" style="27" customWidth="1"/>
@@ -2002,7 +1927,7 @@
     <col min="6" max="16384" width="10.875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="22" customFormat="1">
       <c r="A1" s="22" t="s">
         <v>127</v>
       </c>
@@ -2016,7 +1941,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="23" customFormat="1">
       <c r="A2" s="23">
         <v>1.1000000000000001</v>
       </c>
@@ -2030,7 +1955,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="21">
         <v>1.2</v>
       </c>
@@ -2041,7 +1966,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="31.5">
       <c r="A4" s="21">
         <v>1.3</v>
       </c>
@@ -2052,7 +1977,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="23" customFormat="1" ht="31.5">
       <c r="A5" s="23">
         <v>2.1</v>
       </c>
@@ -2066,7 +1991,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="47.25">
       <c r="A6" s="21">
         <v>2.2000000000000002</v>
       </c>
@@ -2077,7 +2002,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.5">
       <c r="A7" s="21">
         <v>2.2999999999999998</v>
       </c>
@@ -2088,7 +2013,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="31.5">
       <c r="A8" s="21">
         <v>2.4</v>
       </c>
@@ -2099,7 +2024,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="23" customFormat="1" ht="31.5">
       <c r="A9" s="23">
         <v>3.1</v>
       </c>
@@ -2113,7 +2038,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="31.5">
       <c r="A10" s="21">
         <v>3.2</v>
       </c>
@@ -2124,7 +2049,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="31.5">
       <c r="A11" s="21">
         <v>3.3</v>
       </c>
@@ -2135,7 +2060,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="31.5">
       <c r="A12" s="21">
         <v>3.4</v>
       </c>
@@ -2146,7 +2071,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="23" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="23" customFormat="1" ht="47.25">
       <c r="A13" s="24">
         <v>4.0999999999999996</v>
       </c>
@@ -2160,7 +2085,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="31.5">
       <c r="A14" s="21">
         <v>4.2</v>
       </c>
@@ -2171,7 +2096,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="23" customFormat="1" ht="31.5">
       <c r="A15" s="23">
         <v>5.0999999999999996</v>
       </c>
@@ -2185,7 +2110,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="31.5">
       <c r="A16" s="21">
         <v>5.2</v>
       </c>
@@ -2197,31 +2122,27 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20.25" style="32" customWidth="1"/>
     <col min="2" max="2" width="27.625" style="34" customWidth="1"/>
     <col min="3" max="4" width="11" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="20" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
@@ -2235,7 +2156,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="48.75" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>161</v>
       </c>
@@ -2249,7 +2170,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="66.75" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>163</v>
       </c>
@@ -2263,7 +2184,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="31.5">
       <c r="A4" s="32" t="s">
         <v>159</v>
       </c>
@@ -2277,14 +2198,24 @@
         <v>158</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="31.5">
+      <c r="A5" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="32">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
organizing defects found tab
</commit_message>
<xml_diff>
--- a/Documents/Status Updates/StatusSheet.xlsx
+++ b/Documents/Status Updates/StatusSheet.xlsx
@@ -1,38 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Requirements" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Functional Flow Table" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Deliverables" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Issues" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Databases" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Defect Checklist" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Defects Found" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Functional Flow Table" sheetId="2" r:id="rId2"/>
+    <sheet name="Deliverables" sheetId="3" r:id="rId3"/>
+    <sheet name="Issues" sheetId="4" r:id="rId4"/>
+    <sheet name="Databases" sheetId="5" r:id="rId5"/>
+    <sheet name="Defect Checklist" sheetId="6" r:id="rId6"/>
+    <sheet name="Defects Found" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="114210" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C1">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="8"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -43,22 +42,22 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="8"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">See Defect Checklist</t>
+          <t>See Defect Checklist</t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D1">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="8"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -69,7 +68,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="8"/>
             <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
@@ -88,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="178">
   <si>
     <t>Number</t>
   </si>
@@ -603,9 +602,6 @@
     <t>Remove location is giving error when run</t>
   </si>
   <si>
-    <t>Suddent Panel Change</t>
-  </si>
-  <si>
     <t>Choosing locations panel in between changes from a list to a drop down menu without warning</t>
   </si>
   <si>
@@ -616,17 +612,22 @@
   </si>
   <si>
     <t>How to select a location is not obvious</t>
+  </si>
+  <si>
+    <t>Route Calculations 2</t>
+  </si>
+  <si>
+    <t>Sudden Panel Change</t>
+  </si>
+  <si>
+    <t>Choosing more then 13 locations takes too long to process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
-  </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -635,32 +636,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -672,16 +658,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -696,194 +682,419 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.66511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.66511627906977"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="61.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1" s="2">
+    <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +1105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -902,15 +1113,15 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="3">
-      <c r="A3" s="5" t="n">
-        <v>1.1</v>
+    <row r="3" spans="1:3" ht="31.5">
+      <c r="A3" s="5">
+        <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="5">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -918,39 +1129,39 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="6">
-      <c r="A6" s="7" t="n">
+    <row r="6" spans="1:3">
+      <c r="A6" s="7">
         <v>2.1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="7">
-      <c r="A7" s="5" t="n">
-        <v>2.2</v>
+    <row r="7" spans="1:3">
+      <c r="A7" s="5">
+        <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="n">
-        <v>2.3</v>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>2.2999999999999998</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="n">
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
         <v>2.4</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="11">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -958,79 +1169,79 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="12">
-      <c r="A12" s="7" t="n">
+    <row r="12" spans="1:3">
+      <c r="A12" s="7">
         <v>3.1</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="13">
-      <c r="A13" s="7" t="n">
+    <row r="13" spans="1:3" ht="47.25">
+      <c r="A13" s="7">
         <v>3.2</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="14">
-      <c r="A14" s="7" t="n">
+    <row r="14" spans="1:3">
+      <c r="A14" s="7">
         <v>3.3</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="15">
-      <c r="A15" s="7" t="n">
+    <row r="15" spans="1:3">
+      <c r="A15" s="7">
         <v>3.4</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="16">
-      <c r="A16" s="7" t="n">
+    <row r="16" spans="1:3" ht="31.5">
+      <c r="A16" s="7">
         <v>3.5</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="17">
-      <c r="A17" s="7" t="n">
+    <row r="17" spans="1:2">
+      <c r="A17" s="7">
         <v>3.6</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="18">
-      <c r="A18" s="7" t="n">
+    <row r="18" spans="1:2">
+      <c r="A18" s="7">
         <v>3.7</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="19">
-      <c r="A19" s="7" t="n">
+    <row r="19" spans="1:2">
+      <c r="A19" s="7">
         <v>3.8</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="20">
-      <c r="A20" s="7" t="n">
+    <row r="20" spans="1:2">
+      <c r="A20" s="7">
         <v>3.9</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="22" s="4">
+    <row r="22" spans="1:2" s="4" customFormat="1">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -1038,16 +1249,16 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="23">
-      <c r="A23" s="7" t="n">
-        <v>4.1</v>
+    <row r="23" spans="1:2">
+      <c r="A23" s="7">
+        <v>4.0999999999999996</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="24">
-      <c r="A24" s="7" t="n">
+    <row r="24" spans="1:2">
+      <c r="A24" s="7">
         <v>4.2</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1055,38 +1266,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.66511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1255813953488"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1255813953488"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.506976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.66511627906977"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="32.125" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1" s="8">
+    <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1306,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="2" s="12">
+    <row r="2" spans="1:5" s="12" customFormat="1" ht="31.5">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -1114,9 +1317,9 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="3">
-      <c r="A3" s="13" t="n">
-        <v>1.1</v>
+    <row r="3" spans="1:5" ht="31.5">
+      <c r="A3" s="13">
+        <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>33</v>
@@ -1124,15 +1327,15 @@
       <c r="C3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="14" t="n">
-        <v>1.1</v>
+      <c r="D3" s="14">
+        <v>1.1000000000000001</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="78.75" outlineLevel="0" r="4">
-      <c r="A4" s="13" t="n">
+    <row r="4" spans="1:5" ht="78.75">
+      <c r="A4" s="13">
         <v>1.2</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -1141,15 +1344,15 @@
       <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="14">
         <v>1.2</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63" outlineLevel="0" r="5">
-      <c r="A5" s="13" t="n">
+    <row r="5" spans="1:5" ht="63">
+      <c r="A5" s="13">
         <v>1.3</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -1158,14 +1361,14 @@
       <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="14" t="n">
+      <c r="D5" s="14">
         <v>1.3</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="7" s="15">
+    <row r="7" spans="1:5" s="15" customFormat="1" ht="31.5">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1379,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63" outlineLevel="0" r="8">
+    <row r="8" spans="1:5" ht="63">
       <c r="A8" s="13" t="s">
         <v>44</v>
       </c>
@@ -1186,14 +1389,14 @@
       <c r="C8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="14">
         <v>3.1</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="9">
+    <row r="9" spans="1:5" ht="47.25">
       <c r="A9" s="13" t="s">
         <v>48</v>
       </c>
@@ -1203,16 +1406,16 @@
       <c r="C9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="14">
         <v>3.2</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63" outlineLevel="0" r="10">
-      <c r="A10" s="13" t="n">
-        <v>2.2</v>
+    <row r="10" spans="1:5" ht="63">
+      <c r="A10" s="13">
+        <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>51</v>
@@ -1220,16 +1423,16 @@
       <c r="C10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="14">
         <v>2.1</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="11">
-      <c r="A11" s="13" t="n">
-        <v>2.3</v>
+    <row r="11" spans="1:5" ht="47.25">
+      <c r="A11" s="13">
+        <v>2.2999999999999998</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>54</v>
@@ -1237,15 +1440,15 @@
       <c r="C11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="14" t="n">
-        <v>2.2</v>
+      <c r="D11" s="14">
+        <v>2.2000000000000002</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="12">
-      <c r="A12" s="13" t="n">
+    <row r="12" spans="1:5" ht="47.25">
+      <c r="A12" s="13">
         <v>2.4</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -1254,14 +1457,14 @@
       <c r="C12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="14" t="n">
-        <v>2.3</v>
+      <c r="D12" s="14">
+        <v>2.2999999999999998</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="13">
+    <row r="13" spans="1:5" ht="47.25">
       <c r="A13" s="13" t="s">
         <v>60</v>
       </c>
@@ -1271,14 +1474,14 @@
       <c r="C13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="14" t="n">
-        <v>2.3</v>
+      <c r="D13" s="14">
+        <v>2.2999999999999998</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63" outlineLevel="0" r="14">
+    <row r="14" spans="1:5" ht="63">
       <c r="A14" s="13" t="s">
         <v>63</v>
       </c>
@@ -1288,14 +1491,14 @@
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="14" t="n">
-        <v>2.3</v>
+      <c r="D14" s="14">
+        <v>2.2999999999999998</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="15">
+    <row r="15" spans="1:5" ht="47.25">
       <c r="A15" s="13" t="s">
         <v>66</v>
       </c>
@@ -1305,14 +1508,14 @@
       <c r="C15" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="14" t="n">
-        <v>2.3</v>
+      <c r="D15" s="14">
+        <v>2.2999999999999998</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="17" s="15">
+    <row r="17" spans="1:5" s="15" customFormat="1" ht="31.5">
       <c r="A17" s="9" t="s">
         <v>12</v>
       </c>
@@ -1323,8 +1526,8 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63" outlineLevel="0" r="18">
-      <c r="A18" s="13" t="n">
+    <row r="18" spans="1:5" ht="63">
+      <c r="A18" s="13">
         <v>3.1</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1333,15 +1536,15 @@
       <c r="C18" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="14" t="n">
+      <c r="D18" s="14">
         <v>3.2</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="78.75" outlineLevel="0" r="19">
-      <c r="A19" s="13" t="n">
+    <row r="19" spans="1:5" ht="78.75">
+      <c r="A19" s="13">
         <v>3.2</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -1350,15 +1553,15 @@
       <c r="C19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="14" t="n">
-        <v>4.1</v>
+      <c r="D19" s="14">
+        <v>4.0999999999999996</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="20">
-      <c r="A20" s="13" t="n">
+    <row r="20" spans="1:5" ht="31.5">
+      <c r="A20" s="13">
         <v>3.3</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1367,15 +1570,15 @@
       <c r="C20" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="14">
         <v>4.3</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="21">
-      <c r="A21" s="13" t="n">
+    <row r="21" spans="1:5" ht="47.25">
+      <c r="A21" s="13">
         <v>3.4</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -1391,8 +1594,8 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="22">
-      <c r="A22" s="13" t="n">
+    <row r="22" spans="1:5" ht="47.25">
+      <c r="A22" s="13">
         <v>3.5</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -1401,7 +1604,7 @@
       <c r="C22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="14" t="n">
+      <c r="D22" s="14">
         <v>4.2</v>
       </c>
       <c r="E22" s="14" t="s">
@@ -1409,38 +1612,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.5023255813954"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.506976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1" s="16">
+    <row r="1" spans="1:6" s="16" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1460,7 +1655,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2" s="17">
+    <row r="2" spans="1:6" s="17" customFormat="1">
       <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
@@ -1471,37 +1666,37 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:6">
+      <c r="A4">
         <v>1.2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:6">
+      <c r="A5">
         <v>1.3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="7" s="17">
+    <row r="7" spans="1:6" s="17" customFormat="1">
       <c r="A7" s="17" t="s">
         <v>6</v>
       </c>
@@ -1515,96 +1710,88 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:6">
+      <c r="A8">
         <v>2.1</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B10" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:6">
+      <c r="A11">
         <v>2.4</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:6">
+      <c r="A12">
         <v>2.5</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:6">
+      <c r="A13">
         <v>2.6</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1255813953488"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1255813953488"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="46.125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1" s="16">
+    <row r="1" spans="1:5" s="16" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1621,138 +1808,122 @@
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="18" t="n">
+      <c r="E2" s="18">
         <v>41564</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:5">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="18">
         <v>41559</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6186046511628"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4976744186046"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="4">
+    <row r="4" spans="1:4">
       <c r="A4" s="19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.66511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8790697674419"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3720930232558"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6186046511628"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.66511627906977"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="26.875" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="32.375" customWidth="1"/>
+    <col min="5" max="5" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1" s="2">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>119</v>
       </c>
@@ -1766,9 +1937,9 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2" s="20">
-      <c r="A2" s="20" t="n">
-        <v>1.1</v>
+    <row r="2" spans="1:4" s="20" customFormat="1">
+      <c r="A2" s="20">
+        <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>121</v>
@@ -1780,8 +1951,8 @@
         <v>123</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="A3" s="23" t="n">
+    <row r="3" spans="1:4">
+      <c r="A3" s="23">
         <v>1.2</v>
       </c>
       <c r="C3" s="24" t="s">
@@ -1791,8 +1962,8 @@
         <v>125</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="4">
-      <c r="A4" s="23" t="n">
+    <row r="4" spans="1:4" ht="31.5">
+      <c r="A4" s="23">
         <v>1.3</v>
       </c>
       <c r="C4" s="24" t="s">
@@ -1802,8 +1973,8 @@
         <v>127</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="5" s="20">
-      <c r="A5" s="20" t="n">
+    <row r="5" spans="1:4" s="20" customFormat="1" ht="31.5">
+      <c r="A5" s="20">
         <v>2.1</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1816,9 +1987,9 @@
         <v>130</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="6">
-      <c r="A6" s="23" t="n">
-        <v>2.2</v>
+    <row r="6" spans="1:4" ht="47.25">
+      <c r="A6" s="23">
+        <v>2.2000000000000002</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>131</v>
@@ -1827,9 +1998,9 @@
         <v>132</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="7">
-      <c r="A7" s="23" t="n">
-        <v>2.3</v>
+    <row r="7" spans="1:4" ht="31.5">
+      <c r="A7" s="23">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>133</v>
@@ -1838,8 +2009,8 @@
         <v>134</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="8">
-      <c r="A8" s="23" t="n">
+    <row r="8" spans="1:4" ht="31.5">
+      <c r="A8" s="23">
         <v>2.4</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1849,8 +2020,8 @@
         <v>136</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="9" s="20">
-      <c r="A9" s="20" t="n">
+    <row r="9" spans="1:4" s="20" customFormat="1" ht="31.5">
+      <c r="A9" s="20">
         <v>3.1</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -1863,8 +2034,8 @@
         <v>139</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="10">
-      <c r="A10" s="23" t="n">
+    <row r="10" spans="1:4" ht="31.5">
+      <c r="A10" s="23">
         <v>3.2</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -1874,8 +2045,8 @@
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="11">
-      <c r="A11" s="23" t="n">
+    <row r="11" spans="1:4" ht="31.5">
+      <c r="A11" s="23">
         <v>3.3</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -1885,8 +2056,8 @@
         <v>143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="12">
-      <c r="A12" s="23" t="n">
+    <row r="12" spans="1:4" ht="31.5">
+      <c r="A12" s="23">
         <v>3.4</v>
       </c>
       <c r="C12" s="24" t="s">
@@ -1896,9 +2067,9 @@
         <v>145</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="47.25" outlineLevel="0" r="13" s="20">
-      <c r="A13" s="25" t="n">
-        <v>4.1</v>
+    <row r="13" spans="1:4" s="20" customFormat="1" ht="47.25">
+      <c r="A13" s="25">
+        <v>4.0999999999999996</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>146</v>
@@ -1910,8 +2081,8 @@
         <v>148</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="14">
-      <c r="A14" s="23" t="n">
+    <row r="14" spans="1:4" ht="31.5">
+      <c r="A14" s="23">
         <v>4.2</v>
       </c>
       <c r="C14" s="24" t="s">
@@ -1921,9 +2092,9 @@
         <v>150</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="15" s="20">
-      <c r="A15" s="20" t="n">
-        <v>5.1</v>
+    <row r="15" spans="1:4" s="20" customFormat="1" ht="31.5">
+      <c r="A15" s="20">
+        <v>5.0999999999999996</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>151</v>
@@ -1935,8 +2106,8 @@
         <v>153</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="16">
-      <c r="A16" s="23" t="n">
+    <row r="16" spans="1:4" ht="31.5">
+      <c r="A16" s="23">
         <v>5.2</v>
       </c>
       <c r="C16" s="24" t="s">
@@ -1947,37 +2118,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9720930232558"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11"/>
+    <col min="1" max="1" width="20.25" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="1" s="19">
+    <row r="1" spans="1:4" s="19" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -1991,103 +2154,122 @@
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.75" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" ht="48.75" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="C2" s="12">
         <v>2.1</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="66.75" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" ht="66.75" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>161</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="12" t="n">
-        <v>2.2</v>
+      <c r="C3" s="12">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="4">
+    <row r="4" spans="1:4" ht="31.5">
       <c r="A4" s="12" t="s">
         <v>164</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="12">
         <v>3.1</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="31.5" outlineLevel="0" r="5">
+    <row r="5" spans="1:4" ht="31.5">
       <c r="A5" s="28" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="12">
         <v>3.3</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>168</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.05" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:4" ht="32.1" customHeight="1">
+      <c r="A6" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="C6" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>168</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.95" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:4" ht="49.9" customHeight="1">
+      <c r="A7" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="D7" s="0" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="18" customHeight="1">
+      <c r="A8" s="29" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="31.5">
+      <c r="A9" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>163</v>
+      <c r="B9" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>